<commit_message>
update and rerun all data and figures
</commit_message>
<xml_diff>
--- a/data/final_labels_hashed_with_scores.xlsx
+++ b/data/final_labels_hashed_with_scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -965,7 +965,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -4797,7 +4797,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -5993,7 +5993,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -7059,7 +7059,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -7183,7 +7183,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -8241,7 +8241,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -9533,7 +9533,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -10251,7 +10251,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -10491,7 +10491,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -11831,7 +11831,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
@@ -12077,7 +12077,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
@@ -12685,7 +12685,7 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
@@ -13403,7 +13403,7 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I109" t="inlineStr">
@@ -13531,7 +13531,7 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I110" t="inlineStr">
@@ -13775,7 +13775,7 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
@@ -14737,7 +14737,7 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I120" t="inlineStr">
@@ -15095,7 +15095,7 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I123" t="inlineStr">
@@ -15581,7 +15581,7 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I127" t="inlineStr">
@@ -15943,7 +15943,7 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
@@ -16307,7 +16307,7 @@
       </c>
       <c r="H133" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I133" t="inlineStr">
@@ -16909,7 +16909,7 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -17149,7 +17149,7 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I140" t="inlineStr">
@@ -17987,7 +17987,7 @@
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I147" t="inlineStr">
@@ -19651,7 +19651,7 @@
       </c>
       <c r="H161" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
@@ -20013,7 +20013,7 @@
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
@@ -20373,7 +20373,7 @@
       </c>
       <c r="H167" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I167" t="inlineStr">
@@ -20733,7 +20733,7 @@
       </c>
       <c r="H170" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
@@ -20973,7 +20973,7 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I172" t="inlineStr">
@@ -21933,7 +21933,7 @@
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I180" t="inlineStr">
@@ -22657,7 +22657,7 @@
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
@@ -23731,7 +23731,7 @@
       </c>
       <c r="H195" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I195" t="inlineStr">
@@ -24099,7 +24099,7 @@
       </c>
       <c r="H198" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I198" t="inlineStr">
@@ -24345,7 +24345,7 @@
       </c>
       <c r="H200" t="inlineStr">
         <is>
-          <t>Original human-labeled dataset</t>
+          <t>Original human-labeled data</t>
         </is>
       </c>
       <c r="I200" t="inlineStr">
@@ -24552,6 +24552,6 @@
       <c r="AB201" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>